<commit_message>
&&& - №39562 от 06.04.2024 https://numizm.at/ - №89585 от 06.04.2024 https://coinsbolhov.ru/ - Обмен монет, личная вчтреча 06.04.2024  https://www.avito.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Belgium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67960761-A7C7-4EFD-9B77-BFEEEB08ABA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F196AD2-00FB-4C7B-9E16-BB35BE7BEF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="1770" windowWidth="26900" windowHeight="16750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="68">
   <si>
     <t>Year</t>
   </si>
@@ -324,7 +324,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -388,6 +388,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="8">
@@ -551,7 +558,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -645,13 +652,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -842,9 +884,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="5" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1119,7 +1161,7 @@
       <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2267,14 +2309,14 @@
       <c r="G34" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="21">
+      <c r="H34" s="8">
         <v>155000</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J34" s="9" t="s">
-        <v>5</v>
+      <c r="J34" s="35">
+        <v>0</v>
       </c>
       <c r="K34" s="10" t="str">
         <f t="shared" si="3"/>
@@ -2301,14 +2343,14 @@
       <c r="G35" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="21">
+      <c r="H35" s="8">
         <v>130000</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J35" s="9" t="s">
-        <v>5</v>
+      <c r="J35" s="35">
+        <v>0</v>
       </c>
       <c r="K35" s="10" t="str">
         <f t="shared" si="3"/>
@@ -2323,13 +2365,13 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I21 I3:I15">
-    <cfRule type="containsText" dxfId="22" priority="69" operator="containsText" text="*-">
+  <conditionalFormatting sqref="I21 I3:I14">
+    <cfRule type="containsText" dxfId="26" priority="77" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I15 I21">
-    <cfRule type="colorScale" priority="70">
+  <conditionalFormatting sqref="I3:I14 I21">
+    <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2341,11 +2383,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:I20">
-    <cfRule type="containsText" dxfId="21" priority="67" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="25" priority="75" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:I20">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:I27 J3:J27 J29">
+    <cfRule type="containsText" dxfId="24" priority="73" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:I27 J3:J27 J29">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="containsText" dxfId="23" priority="67" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2357,13 +2433,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22:I27 J3:J27 J29">
-    <cfRule type="containsText" dxfId="20" priority="65" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22:I27 J3:J27 J29">
-    <cfRule type="colorScale" priority="66">
+  <conditionalFormatting sqref="J28">
+    <cfRule type="containsText" dxfId="22" priority="63" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J28))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2374,13 +2450,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="containsText" dxfId="19" priority="59" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="colorScale" priority="60">
+  <conditionalFormatting sqref="I28">
+    <cfRule type="containsText" dxfId="21" priority="61" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I28))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2391,13 +2467,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28">
-    <cfRule type="containsText" dxfId="18" priority="55" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J28))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J28">
-    <cfRule type="colorScale" priority="56">
+  <conditionalFormatting sqref="I31">
+    <cfRule type="containsText" dxfId="20" priority="49" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2408,13 +2484,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="containsText" dxfId="17" priority="53" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I28))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I28">
-    <cfRule type="colorScale" priority="54">
+  <conditionalFormatting sqref="I30">
+    <cfRule type="containsText" dxfId="19" priority="45" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2425,13 +2501,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="containsText" dxfId="16" priority="41" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I31))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="colorScale" priority="42">
+  <conditionalFormatting sqref="I33">
+    <cfRule type="containsText" dxfId="18" priority="39" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2442,12 +2518,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
-    <cfRule type="containsText" dxfId="15" priority="37" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I30))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I30">
+  <conditionalFormatting sqref="I32">
+    <cfRule type="containsText" dxfId="17" priority="37" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2459,12 +2535,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
-    <cfRule type="containsText" dxfId="14" priority="31" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I33))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33">
+  <conditionalFormatting sqref="I35">
+    <cfRule type="containsText" dxfId="16" priority="31" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I35))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2476,12 +2552,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="containsText" dxfId="13" priority="29" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I32))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
+  <conditionalFormatting sqref="I34">
+    <cfRule type="containsText" dxfId="15" priority="29" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I34))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2493,12 +2569,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I35))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
+  <conditionalFormatting sqref="J33">
+    <cfRule type="containsText" dxfId="14" priority="25" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30">
+    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2510,12 +2603,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
-    <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I34))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34">
+  <conditionalFormatting sqref="J31">
+    <cfRule type="containsText" dxfId="12" priority="21" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2527,46 +2620,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33">
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J33))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J33">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30">
-    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J30))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
-    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J31))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
+  <conditionalFormatting sqref="I16">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2578,12 +2637,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
+  <conditionalFormatting sqref="I17">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J34))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2595,12 +2671,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J35))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
+  <conditionalFormatting sqref="J34">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J34))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2612,12 +2688,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+  <conditionalFormatting sqref="J35">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J35))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J35">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2629,29 +2705,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J32))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
+  <conditionalFormatting sqref="I15">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2677,7 +2736,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
### - №10013435 от 26.04.2024 https://newcoin.ru/ - № 108162 от 22.04.2024https://eurocoin.ru/ - № 1270782786 от 27.04.2024 https://2euro.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Belgium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52874BB-94CB-47FC-95EF-C6C555CAFE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FA8BC2-EC9F-4AB0-89E5-A77970C9492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1110" windowWidth="28720" windowHeight="19550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -1242,7 +1242,7 @@
       <pane xSplit="12" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1410,7 +1410,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>3</v>
@@ -1624,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="J11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>3</v>
@@ -1696,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="J13" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
&&& - №10013533 от 14.05.2024 https://newcoin.ru/ - №67904280 от 24.05.2024 https://meshok.net/ - №52355 от 14.05.2024 https://proof.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Belgium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FA8BC2-EC9F-4AB0-89E5-A77970C9492D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8792C7CF-5EC0-4BAC-8D15-91EA7F901148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1242,7 +1242,7 @@
       <pane xSplit="12" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1766,7 +1766,7 @@
         <v>3</v>
       </c>
       <c r="J15" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>3</v>
@@ -1875,7 +1875,7 @@
         <v>3</v>
       </c>
       <c r="J18" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>3</v>
@@ -1947,7 +1947,7 @@
         <v>3</v>
       </c>
       <c r="J20" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>3</v>
@@ -2017,7 +2017,7 @@
         <v>3</v>
       </c>
       <c r="J22" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
&& - №11434 от 05.06.2024 https://2eurostore.ru/ - №68029073 от 28.05.2024 https://meshok.net/ - №68076146 от 30.05.2024 https://meshok.net/ - №67903344 от 23.05.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Belgium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8792C7CF-5EC0-4BAC-8D15-91EA7F901148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938A1979-4AC1-492A-A23F-C8F0CCD264EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="74">
   <si>
     <t>Year</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>Erasmus Programme</t>
+  </si>
+  <si>
+    <t>Fight Against Cancer in Belgium</t>
   </si>
 </sst>
 </file>
@@ -686,7 +689,23 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -965,9 +984,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="3" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1236,13 +1255,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="12" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2052,7 +2071,7 @@
         <v>3</v>
       </c>
       <c r="J23" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>3</v>
@@ -2090,7 +2109,7 @@
         <v>3</v>
       </c>
       <c r="K24" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="10" t="str">
         <f t="shared" si="1"/>
@@ -2160,7 +2179,7 @@
         <v>3</v>
       </c>
       <c r="K26" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="10" t="str">
         <f t="shared" si="1"/>
@@ -2195,7 +2214,7 @@
         <v>3</v>
       </c>
       <c r="K27" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="10" t="str">
         <f t="shared" si="1"/>
@@ -2265,7 +2284,7 @@
         <v>3</v>
       </c>
       <c r="K29" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L29" s="10" t="str">
         <f t="shared" si="1"/>
@@ -2300,7 +2319,7 @@
         <v>3</v>
       </c>
       <c r="K30" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="10" t="str">
         <f t="shared" ref="L30:L31" si="2">IF(OR(AND(J30&gt;1,J30&lt;&gt;"-"),AND(K30&gt;1,K30&lt;&gt;"-")),"Can exchange","")</f>
@@ -2335,7 +2354,7 @@
         <v>3</v>
       </c>
       <c r="K31" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2442,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="K34" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34" s="10" t="str">
         <f t="shared" si="3"/>
@@ -2477,7 +2496,7 @@
         <v>3</v>
       </c>
       <c r="K35" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" s="10" t="str">
         <f t="shared" si="3"/>
@@ -2512,10 +2531,45 @@
         <v>3</v>
       </c>
       <c r="K36" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36" s="10" t="str">
         <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="19">
+        <v>2024</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" s="21">
+        <v>130000</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K37" s="26">
+        <v>1</v>
+      </c>
+      <c r="L37" s="10" t="str">
+        <f t="shared" ref="L37" si="4">IF(OR(AND(J37&gt;1,J37&lt;&gt;"-"),AND(K37&gt;1,K37&lt;&gt;"-")),"Can exchange","")</f>
         <v/>
       </c>
     </row>
@@ -2528,11 +2582,45 @@
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="J21 J3:J14">
+    <cfRule type="containsText" dxfId="35" priority="107" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J14 J21">
+    <cfRule type="colorScale" priority="108">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="containsText" dxfId="34" priority="105" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="colorScale" priority="106">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24:J27 K3:K23 K25">
     <cfRule type="containsText" dxfId="33" priority="103" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(J3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J14 J21">
+  <conditionalFormatting sqref="J24:J27 K3:K23 K25">
     <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2544,13 +2632,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J19">
-    <cfRule type="containsText" dxfId="32" priority="101" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J19))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J19">
-    <cfRule type="colorScale" priority="102">
+  <conditionalFormatting sqref="J29">
+    <cfRule type="containsText" dxfId="32" priority="97" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="colorScale" priority="98">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2561,29 +2649,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:J27 K3:K23 K25">
-    <cfRule type="containsText" dxfId="31" priority="99" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J24:J27 K3:K23 K25">
-    <cfRule type="colorScale" priority="100">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29">
-    <cfRule type="containsText" dxfId="30" priority="93" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29">
+  <conditionalFormatting sqref="K28">
+    <cfRule type="containsText" dxfId="31" priority="93" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K28))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28">
     <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2595,13 +2666,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
-    <cfRule type="containsText" dxfId="29" priority="89" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K28))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
-    <cfRule type="colorScale" priority="90">
+  <conditionalFormatting sqref="J28">
+    <cfRule type="containsText" dxfId="30" priority="91" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J28))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28">
+    <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2612,13 +2683,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28">
-    <cfRule type="containsText" dxfId="28" priority="87" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J28))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J28">
-    <cfRule type="colorScale" priority="88">
+  <conditionalFormatting sqref="J31">
+    <cfRule type="containsText" dxfId="29" priority="79" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2629,12 +2700,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
-    <cfRule type="containsText" dxfId="27" priority="75" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J31))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
+  <conditionalFormatting sqref="J30">
+    <cfRule type="containsText" dxfId="28" priority="75" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2646,13 +2717,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J30">
-    <cfRule type="containsText" dxfId="26" priority="71" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J30))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J30">
-    <cfRule type="colorScale" priority="72">
+  <conditionalFormatting sqref="J33">
+    <cfRule type="containsText" dxfId="27" priority="69" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33">
+    <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2663,13 +2734,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33">
-    <cfRule type="containsText" dxfId="25" priority="65" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J33))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J33">
-    <cfRule type="colorScale" priority="66">
+  <conditionalFormatting sqref="J32">
+    <cfRule type="containsText" dxfId="26" priority="67" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2680,13 +2751,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
-    <cfRule type="containsText" dxfId="24" priority="63" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J32))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
-    <cfRule type="colorScale" priority="64">
+  <conditionalFormatting sqref="J35">
+    <cfRule type="containsText" dxfId="25" priority="61" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J35))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J35">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2697,13 +2768,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
-    <cfRule type="containsText" dxfId="23" priority="57" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J35))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
-    <cfRule type="colorScale" priority="58">
+  <conditionalFormatting sqref="J34">
+    <cfRule type="containsText" dxfId="24" priority="59" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J34))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2714,12 +2785,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
-    <cfRule type="containsText" dxfId="22" priority="55" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J34))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J34">
+  <conditionalFormatting sqref="K33">
+    <cfRule type="containsText" dxfId="23" priority="55" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2731,13 +2802,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
-    <cfRule type="containsText" dxfId="21" priority="51" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K33))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
-    <cfRule type="colorScale" priority="52">
+  <conditionalFormatting sqref="J16">
+    <cfRule type="containsText" dxfId="22" priority="43" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2748,12 +2819,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16">
+  <conditionalFormatting sqref="J17">
+    <cfRule type="containsText" dxfId="21" priority="41" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
     <cfRule type="containsText" dxfId="20" priority="39" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J16">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K32">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2765,12 +2853,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
+  <conditionalFormatting sqref="K34">
     <cfRule type="containsText" dxfId="19" priority="37" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J17))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K34))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K34">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2782,12 +2870,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+  <conditionalFormatting sqref="K35">
     <cfRule type="containsText" dxfId="18" priority="35" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K32))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K35))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2799,13 +2887,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
-    <cfRule type="containsText" dxfId="17" priority="33" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K34))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K34">
-    <cfRule type="colorScale" priority="34">
+  <conditionalFormatting sqref="J15">
+    <cfRule type="containsText" dxfId="17" priority="29" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2816,13 +2904,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
-    <cfRule type="containsText" dxfId="16" priority="31" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K35))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="J18">
+    <cfRule type="containsText" dxfId="16" priority="27" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -2833,12 +2921,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
+  <conditionalFormatting sqref="J20">
     <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J20))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2850,12 +2938,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
+  <conditionalFormatting sqref="J22">
     <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2867,12 +2955,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J20">
+  <conditionalFormatting sqref="J23">
     <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J20))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J20">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2884,12 +2972,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J22">
+  <conditionalFormatting sqref="K24">
     <cfRule type="containsText" dxfId="12" priority="19" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J22))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J22">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2901,12 +2989,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J23">
+  <conditionalFormatting sqref="K26">
     <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J23))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J23">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K26))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K26">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2918,12 +3006,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
+  <conditionalFormatting sqref="K27">
     <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K24))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2935,12 +3023,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K29">
     <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K26))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2952,12 +3040,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="K30">
     <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K27))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2969,12 +3057,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+  <conditionalFormatting sqref="K31">
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K29))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K29">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2986,12 +3074,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+  <conditionalFormatting sqref="J36">
     <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K30))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J36))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3003,12 +3091,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
+  <conditionalFormatting sqref="K36">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K31))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K36))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3020,12 +3108,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(J36))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J36">
+  <conditionalFormatting sqref="J37">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(J37))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -3037,12 +3125,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(K36))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K36">
+  <conditionalFormatting sqref="K37">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(K37))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K37">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>

</xml_diff>

<commit_message>
&& - 19387 от 16.06.2025 https://2eurostore.ru/ - 20133 от 20.07.2025 https://2eurostore.ru/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Belgium/#EURO#Belgium#Commemorative#[2005-present]#UNC%varieties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Belgium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE85790-39F9-456B-8B1F-EE7867311FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C755C126-DDD7-4FC5-8138-E09DB7FD5CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2960" yWindow="2960" windowWidth="33150" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -128,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="76">
   <si>
     <t>Year</t>
   </si>
@@ -355,6 +358,9 @@
   </si>
   <si>
     <t>Subtype_5#Special_distinctions_1</t>
+  </si>
+  <si>
+    <t>Circuit de Spa-Francorchamps</t>
   </si>
 </sst>
 </file>
@@ -1336,7 +1342,7 @@
       <pane xSplit="12" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2687,21 +2693,31 @@
       <c r="A39" s="19">
         <v>2025</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="7"/>
+      <c r="D39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="G39" s="7"/>
       <c r="H39" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="I39" s="21"/>
+      <c r="I39" s="21">
+        <v>155000</v>
+      </c>
       <c r="J39" s="9" t="s">
         <v>3</v>
       </c>
       <c r="K39" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="10" t="str">
         <f t="shared" ref="L39" si="5">IF(OR(AND(J39&gt;1,J39&lt;&gt;"-"),AND(K39&gt;1,K39&lt;&gt;"-")),"Can exchange","")</f>
@@ -3376,7 +3392,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>